<commit_message>
Adapt generics to getter / setter.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectTsClassStructure.xlsx
+++ b/meta/program/BlancoValueObjectTsClassStructure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3791C4-E9D2-0B40-A8E3-4ED8D6262722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552B278D-A0C5-8B46-9E50-95CCA6B0A506}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28300" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16360" yWindow="920" windowWidth="28300" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -986,47 +986,47 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1441,7 +1441,7 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="A43" sqref="A43:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1636,24 +1636,24 @@
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="58" t="s">
+      <c r="A19" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="52"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="54"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="58"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="52"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="54"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
@@ -1695,30 +1695,30 @@
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A25" s="58" t="s">
+      <c r="A25" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="53" t="s">
+      <c r="C25" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="53" t="s">
+      <c r="D25" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="53" t="s">
+      <c r="E25" s="48" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="58"/>
-      <c r="B26" s="58"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
       <c r="F26" s="9"/>
       <c r="G26"/>
     </row>
@@ -1766,10 +1766,10 @@
         <v>33</v>
       </c>
       <c r="D29" s="40"/>
-      <c r="E29" s="56" t="s">
+      <c r="E29" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="F29" s="57"/>
+      <c r="F29" s="58"/>
       <c r="G29"/>
     </row>
     <row r="30" spans="1:7" ht="15">
@@ -1804,10 +1804,10 @@
       <c r="D31" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E31" s="49" t="s">
+      <c r="E31" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="F31" s="50"/>
+      <c r="F31" s="52"/>
       <c r="G31"/>
     </row>
     <row r="32" spans="1:7" ht="15">
@@ -1824,10 +1824,10 @@
       <c r="D32" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="49" t="s">
+      <c r="E32" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="F32" s="50"/>
+      <c r="F32" s="52"/>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:7" ht="15">
@@ -1844,10 +1844,10 @@
       <c r="D33" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E33" s="49" t="s">
+      <c r="E33" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="50"/>
+      <c r="F33" s="52"/>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" ht="15">
@@ -1864,10 +1864,10 @@
       <c r="D34" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="54" t="s">
+      <c r="E34" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="F34" s="55"/>
+      <c r="F34" s="56"/>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" ht="15">
@@ -1884,10 +1884,10 @@
       <c r="D35" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="49" t="s">
+      <c r="E35" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F35" s="50"/>
+      <c r="F35" s="52"/>
       <c r="G35"/>
     </row>
     <row r="36" spans="1:7" ht="15">
@@ -1904,10 +1904,10 @@
       <c r="D36" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="49" t="s">
+      <c r="E36" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="F36" s="50"/>
+      <c r="F36" s="52"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" ht="15">
@@ -1924,10 +1924,10 @@
       <c r="D37" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E37" s="49" t="s">
+      <c r="E37" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="F37" s="50"/>
+      <c r="F37" s="52"/>
       <c r="G37"/>
     </row>
     <row r="38" spans="1:7" ht="15">
@@ -1944,10 +1944,10 @@
       <c r="D38" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="49" t="s">
+      <c r="E38" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="F38" s="50"/>
+      <c r="F38" s="52"/>
       <c r="G38"/>
     </row>
     <row r="39" spans="1:7" ht="15">
@@ -1964,10 +1964,10 @@
       <c r="D39" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="49" t="s">
+      <c r="E39" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="F39" s="50"/>
+      <c r="F39" s="52"/>
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7" ht="15">
@@ -1984,10 +1984,10 @@
       <c r="D40" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="49" t="s">
+      <c r="E40" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="50"/>
+      <c r="F40" s="52"/>
       <c r="G40"/>
     </row>
     <row r="41" spans="1:7" ht="15">
@@ -2004,10 +2004,10 @@
       <c r="D41" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E41" s="49" t="s">
+      <c r="E41" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="50"/>
+      <c r="F41" s="52"/>
       <c r="G41"/>
     </row>
     <row r="42" spans="1:7" ht="15">
@@ -2024,10 +2024,10 @@
       <c r="D42" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="49" t="s">
+      <c r="E42" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="F42" s="50"/>
+      <c r="F42" s="52"/>
       <c r="G42"/>
     </row>
     <row r="43" spans="1:7" ht="15">
@@ -2044,10 +2044,10 @@
       <c r="D43" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="49" t="s">
+      <c r="E43" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="F43" s="50"/>
+      <c r="F43" s="52"/>
       <c r="G43"/>
     </row>
     <row r="44" spans="1:7" ht="15">
@@ -2062,10 +2062,10 @@
         <v>33</v>
       </c>
       <c r="D44" s="40"/>
-      <c r="E44" s="49" t="s">
+      <c r="E44" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="F44" s="50"/>
+      <c r="F44" s="52"/>
       <c r="G44"/>
     </row>
     <row r="45" spans="1:7" ht="45" customHeight="1">
@@ -2082,10 +2082,10 @@
       <c r="D45" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E45" s="49" t="s">
+      <c r="E45" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="F45" s="51"/>
+      <c r="F45" s="53"/>
       <c r="G45"/>
     </row>
     <row r="46" spans="1:7" ht="45">
@@ -2102,10 +2102,10 @@
       <c r="D46" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="E46" s="49" t="s">
+      <c r="E46" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="F46" s="51"/>
+      <c r="F46" s="53"/>
       <c r="G46"/>
     </row>
     <row r="47" spans="1:7" ht="15">
@@ -2120,10 +2120,10 @@
         <v>63</v>
       </c>
       <c r="D47" s="40"/>
-      <c r="E47" s="49" t="s">
+      <c r="E47" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="F47" s="51"/>
+      <c r="F47" s="53"/>
       <c r="G47"/>
     </row>
     <row r="48" spans="1:7">
@@ -2140,10 +2140,10 @@
       <c r="D48" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="E48" s="49" t="s">
+      <c r="E48" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="F48" s="50"/>
+      <c r="F48" s="52"/>
       <c r="G48"/>
     </row>
     <row r="49" spans="1:7" ht="14" customHeight="1">
@@ -2151,8 +2151,8 @@
       <c r="B49" s="22"/>
       <c r="C49" s="44"/>
       <c r="D49" s="44"/>
-      <c r="E49" s="47"/>
-      <c r="F49" s="48"/>
+      <c r="E49" s="59"/>
+      <c r="F49" s="60"/>
       <c r="G49"/>
     </row>
     <row r="50" spans="1:7">
@@ -2160,14 +2160,17 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E43:F43"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="E19:E20"/>
@@ -2179,17 +2182,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations disablePrompts="1" count="6">

</xml_diff>